<commit_message>
mean and error of results implemented
</commit_message>
<xml_diff>
--- a/protect_baltic/src/data/example/exampleResults.xlsx
+++ b/protect_baltic/src/data/example/exampleResults.xlsx
@@ -7,13 +7,18 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PressureLevels" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="TPLLevels" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TPLReductions" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="RequiredReductionsForGES" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="MeasureEffects" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="ActivityContributions" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="PressureContributions" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="PressureMean" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="PressureError" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TPLMean" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TPLError" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="ThresholdsMean" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ThresholdsError" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="MeasureEffectsMean" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="MeasureEffectsError" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="ActivityContributionsMean" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="ActivityContributionsError" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="PressureContributionsMean" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="PressureContributionsError" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,10 +462,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6454648000000001</v>
+        <v>0.7113447999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5105919999999999</v>
+        <v>0.587032</v>
       </c>
     </row>
     <row r="3">
@@ -468,10 +473,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5893512439999999</v>
+        <v>0.6090166832999999</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4892217599999999</v>
+        <v>0.497857232</v>
       </c>
     </row>
     <row r="4">
@@ -479,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.60415</v>
+        <v>0.5243646999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4694</v>
+        <v>0.4316391999999999</v>
       </c>
     </row>
     <row r="5">
@@ -490,10 +495,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9649</v>
+        <v>0.9643600000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9064</v>
+        <v>0.90496</v>
       </c>
     </row>
     <row r="6">
@@ -501,10 +506,607 @@
         <v>31</v>
       </c>
       <c r="B6" t="n">
-        <v>0.86</v>
+        <v>0.8892</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Pressure</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>area_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>contribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.009833094909913095</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01503795225662456</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.008067272112637899</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.01197886410695183</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="n">
+        <v>31</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.01229759062744309</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>11</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0004063846268960041</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>11</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.001230300045353961</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.004110111131920906</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.005232694204459066</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.01503067823943486</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01353821583642829</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>State</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pressure</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>area_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>contribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.6733078578107896</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.2108566532035205</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1158354889856898</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.8322149894900376</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1677850105099625</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.634789609326299</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.2504022498797214</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1148081407939794</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.8348339085354549</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.1651660914645451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>State</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pressure</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>area_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>contribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.009317492382900052</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.009601053342045479</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.001615633967050586</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.002500937145622117</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.002500937145622084</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.00792795462968642</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.006422176609741857</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.001920979224065383</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.004557601564557755</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.004557601564557695</v>
       </c>
     </row>
   </sheetData>
@@ -518,7 +1120,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,10 +1146,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5899522796862745</v>
+        <v>0.01215713906410551</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4683781678431373</v>
+        <v>0.01224750253725224</v>
       </c>
     </row>
     <row r="3">
@@ -555,10 +1157,43 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5951528409203539</v>
+        <v>0.009199572210542085</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4854296028070174</v>
+        <v>0.01164177826554736</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.01409361249806293</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.008217210206227737</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>11</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0005400000000000001</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.001439999999999995</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.01639566338327845</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -598,10 +1233,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4100477203137255</v>
+        <v>0.6126383934131945</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5316218321568627</v>
+        <v>0.5028670935072653</v>
       </c>
     </row>
     <row r="3">
@@ -609,10 +1244,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.4048471590796461</v>
+        <v>0.6217541993486156</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5145703971929826</v>
+        <v>0.50428426593076</v>
       </c>
     </row>
   </sheetData>
@@ -652,10 +1287,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.51</v>
+        <v>0.008598410457848394</v>
       </c>
       <c r="C2" t="n">
-        <v>0.49</v>
+        <v>0.007148879998090671</v>
       </c>
     </row>
     <row r="3">
@@ -663,10 +1298,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.88</v>
+        <v>0.009100028149991798</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8200000000000001</v>
+        <v>0.01045132217958939</v>
       </c>
     </row>
   </sheetData>
@@ -675,6 +1310,114 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5110000000000001</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.511</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5399999999999999</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.575</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01303414319734478</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.01369914839202302</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.08481352093465602</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.08709190547921203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -729,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.52</v>
+        <v>0.411</v>
       </c>
     </row>
     <row r="3">
@@ -746,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.77</v>
+        <v>0.5870000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -763,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.31</v>
+        <v>0.355</v>
       </c>
     </row>
     <row r="5">
@@ -780,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.32</v>
+        <v>0.226</v>
       </c>
     </row>
     <row r="6">
@@ -797,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.37</v>
+        <v>0.349</v>
       </c>
     </row>
     <row r="7">
@@ -814,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.35</v>
+        <v>0.277</v>
       </c>
     </row>
     <row r="8">
@@ -831,7 +1574,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.39</v>
+        <v>0.396</v>
       </c>
     </row>
     <row r="9">
@@ -848,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.35</v>
+        <v>0.426</v>
       </c>
     </row>
     <row r="10">
@@ -865,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11">
@@ -882,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7000000000000001</v>
+        <v>0.66</v>
       </c>
     </row>
   </sheetData>
@@ -890,7 +1633,223 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>measure</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pressure</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>state</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>reduction</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0267685553505518</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.03732886878066954</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.01916304313573974</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.02840970100355002</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.04249052181892386</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>31</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.04098915845819612</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>11</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.005999999999999998</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.01343296111973992</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.02586288632169443</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.01960725489313699</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -937,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3802915356499688</v>
+        <v>0.4361746830281742</v>
       </c>
     </row>
     <row r="3">
@@ -951,7 +1910,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2165956380045124</v>
+        <v>0.3157890423588068</v>
       </c>
     </row>
     <row r="4">
@@ -965,7 +1924,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5176899974440369</v>
+        <v>0.5377910482969257</v>
       </c>
     </row>
     <row r="5">
@@ -979,7 +1938,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4726317978987688</v>
+        <v>0.4976488234378473</v>
       </c>
     </row>
     <row r="6">
@@ -993,7 +1952,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3023255813953488</v>
+        <v>0.3231985276969553</v>
       </c>
     </row>
     <row r="7">
@@ -1007,7 +1966,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2745362213700901</v>
+        <v>0.2741279449337248</v>
       </c>
     </row>
     <row r="8">
@@ -1021,7 +1980,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2277140335392762</v>
+        <v>0.2264675296970426</v>
       </c>
     </row>
     <row r="9">
@@ -1035,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2277928508113916</v>
+        <v>0.2153667956960144</v>
       </c>
     </row>
     <row r="10">
@@ -1049,7 +2008,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>0.220758782274934</v>
+        <v>0.1994960199631916</v>
       </c>
     </row>
     <row r="11">
@@ -1063,7 +2022,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5034345775055865</v>
+        <v>0.4242565689366816</v>
       </c>
     </row>
     <row r="12">
@@ -1077,188 +2036,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3608862377503196</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>State</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>pressure</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>area_id</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>contribution</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.6469569066904042</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.2355158917748217</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.1175272015347741</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.8412759682689286</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.1587240317310716</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.5921834597859824</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.2849339954500048</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.1228825447640127</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.8575242125483313</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>2</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.142475787451669</v>
+        <v>0.3026595020213364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
state / pressure level plots
</commit_message>
<xml_diff>
--- a/protect_baltic/src/data/example/exampleResults.xlsx
+++ b/protect_baltic/src/data/example/exampleResults.xlsx
@@ -462,10 +462,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.71011378</v>
+        <v>0.7113447999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5863311999999999</v>
+        <v>0.587032</v>
       </c>
     </row>
     <row r="3">
@@ -473,10 +473,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6086373608</v>
+        <v>0.6096956486</v>
       </c>
       <c r="C3" t="n">
-        <v>0.498257232</v>
+        <v>0.499592544</v>
       </c>
     </row>
     <row r="4">
@@ -484,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5256722999999999</v>
+        <v>0.5250332</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4327927999999999</v>
+        <v>0.4322551999999999</v>
       </c>
     </row>
     <row r="5">
@@ -495,10 +495,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>0.96445</v>
+        <v>0.9643600000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9052</v>
+        <v>0.90496</v>
       </c>
     </row>
     <row r="6">
@@ -506,7 +506,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8888</v>
+        <v>0.8904</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -564,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.009999224065384022</v>
+        <v>0.009833094909913095</v>
       </c>
     </row>
     <row r="3">
@@ -578,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01514014868299096</v>
+        <v>0.01503795225662456</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.008367800442221148</v>
+        <v>0.008203096626521822</v>
       </c>
     </row>
     <row r="5">
@@ -606,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01247006319020318</v>
+        <v>0.01231084081331761</v>
       </c>
     </row>
     <row r="6">
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0122240578778499</v>
+        <v>0.01217620155530652</v>
       </c>
     </row>
     <row r="7">
@@ -634,7 +634,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0004070463275489701</v>
+        <v>0.0004063846268960041</v>
       </c>
     </row>
     <row r="8">
@@ -648,7 +648,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>0.001232498433420237</v>
+        <v>0.001230300045353961</v>
       </c>
     </row>
     <row r="9">
@@ -662,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.004238734954778736</v>
+        <v>0.004203198890535038</v>
       </c>
     </row>
     <row r="10">
@@ -676,7 +676,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>0.005363794299581409</v>
+        <v>0.005436662274549129</v>
       </c>
     </row>
     <row r="11">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01496424748634719</v>
+        <v>0.01532015968747565</v>
       </c>
     </row>
     <row r="12">
@@ -704,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01358443911296384</v>
+        <v>0.01390568315370264</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +761,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.672675323469343</v>
+        <v>0.6727549802662831</v>
       </c>
     </row>
     <row r="3">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.2114822835219262</v>
+        <v>0.2113769774816732</v>
       </c>
     </row>
     <row r="4">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.1158423930087307</v>
+        <v>0.1158680422520436</v>
       </c>
     </row>
     <row r="5">
@@ -809,7 +809,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.8323679504139248</v>
+        <v>0.83236812445981</v>
       </c>
     </row>
     <row r="6">
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.1676320495860753</v>
+        <v>0.1676318755401902</v>
       </c>
     </row>
     <row r="7">
@@ -841,7 +841,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.634064172919435</v>
+        <v>0.6343263002050215</v>
       </c>
     </row>
     <row r="8">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2510567781553593</v>
+        <v>0.250559293105184</v>
       </c>
     </row>
     <row r="9">
@@ -873,7 +873,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.1148790489252055</v>
+        <v>0.1151144066897944</v>
       </c>
     </row>
     <row r="10">
@@ -889,7 +889,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.8350437928856878</v>
+        <v>0.8352891734856789</v>
       </c>
     </row>
     <row r="11">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.1649562071143122</v>
+        <v>0.1647108265143212</v>
       </c>
     </row>
   </sheetData>
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.009290381553297034</v>
+        <v>0.009322458761353375</v>
       </c>
     </row>
     <row r="3">
@@ -978,7 +978,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.009621570204738958</v>
+        <v>0.009657071528972789</v>
       </c>
     </row>
     <row r="4">
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.001580350035827439</v>
+        <v>0.001632923101321011</v>
       </c>
     </row>
     <row r="5">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.002417280887037189</v>
+        <v>0.002487358973910752</v>
       </c>
     </row>
     <row r="6">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.002417280887037153</v>
+        <v>0.002487358973910721</v>
       </c>
     </row>
     <row r="7">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.00798978595289032</v>
+        <v>0.008045319065386506</v>
       </c>
     </row>
     <row r="8">
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.006445390933996853</v>
+        <v>0.006492128472678519</v>
       </c>
     </row>
     <row r="9">
@@ -1074,7 +1074,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.001978516649907895</v>
+        <v>0.001944735896859549</v>
       </c>
     </row>
     <row r="10">
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.004686438762621713</v>
+        <v>0.004606348893236272</v>
       </c>
     </row>
     <row r="11">
@@ -1106,7 +1106,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.004686438762621669</v>
+        <v>0.004606348893236218</v>
       </c>
     </row>
   </sheetData>
@@ -1146,10 +1146,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.01226934568754177</v>
+        <v>0.01215713906410551</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01229391201530254</v>
+        <v>0.01224750253725224</v>
       </c>
     </row>
     <row r="3">
@@ -1157,10 +1157,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.009586075507672428</v>
+        <v>0.009344207559866452</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01216651307444211</v>
+        <v>0.01188433385159427</v>
       </c>
     </row>
     <row r="4">
@@ -1168,10 +1168,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.01419854961845674</v>
+        <v>0.01444813800214024</v>
       </c>
       <c r="C4" t="n">
-        <v>0.008318550510488921</v>
+        <v>0.008498693898084178</v>
       </c>
     </row>
     <row r="5">
@@ -1179,10 +1179,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0005408326913195982</v>
+        <v>0.0005400000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.001442220510185591</v>
+        <v>0.001439999999999995</v>
       </c>
     </row>
     <row r="6">
@@ -1190,7 +1190,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="n">
-        <v>0.016295057191949</v>
+        <v>0.01626666666666667</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -1233,10 +1233,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6121718024878179</v>
+        <v>0.6131565049253417</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5028994885693594</v>
+        <v>0.503246469473797</v>
       </c>
     </row>
     <row r="3">
@@ -1244,10 +1244,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.621250581149451</v>
+        <v>0.6223306234372835</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5045360905965837</v>
+        <v>0.5057565134872066</v>
       </c>
     </row>
   </sheetData>
@@ -1287,10 +1287,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.008821392431496418</v>
+        <v>0.008708835448271574</v>
       </c>
       <c r="C2" t="n">
-        <v>0.007250804732260575</v>
+        <v>0.007163802701522741</v>
       </c>
     </row>
     <row r="3">
@@ -1298,10 +1298,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.009503025987692421</v>
+        <v>0.00923368994353385</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01090936179063572</v>
+        <v>0.01066197055715727</v>
       </c>
     </row>
   </sheetData>
@@ -1472,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.414</v>
+        <v>0.411</v>
       </c>
     </row>
     <row r="3">
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5860000000000001</v>
+        <v>0.5870000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -1506,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.356</v>
+        <v>0.354</v>
       </c>
     </row>
     <row r="5">
@@ -1540,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.345</v>
+        <v>0.344</v>
       </c>
     </row>
     <row r="7">
@@ -1557,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.278</v>
+        <v>0.274</v>
       </c>
     </row>
     <row r="8">
@@ -1574,7 +1574,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.395</v>
+        <v>0.396</v>
       </c>
     </row>
     <row r="9">
@@ -1591,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.425</v>
+        <v>0.424</v>
       </c>
     </row>
     <row r="10">
@@ -1608,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5980000000000001</v>
+        <v>0.599</v>
       </c>
     </row>
     <row r="11">
@@ -1625,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.658</v>
+        <v>0.659</v>
       </c>
     </row>
   </sheetData>
@@ -1688,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02704728370013439</v>
+        <v>0.0267685553505518</v>
       </c>
     </row>
     <row r="3">
@@ -1705,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03748184745832159</v>
+        <v>0.03732886878066954</v>
       </c>
     </row>
     <row r="4">
@@ -1722,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02045048220023729</v>
+        <v>0.01967513941783161</v>
       </c>
     </row>
     <row r="5">
@@ -1756,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0441021541423999</v>
+        <v>0.04292629341868066</v>
       </c>
     </row>
     <row r="7">
@@ -1773,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0407376429798725</v>
+        <v>0.04066666666666666</v>
       </c>
     </row>
     <row r="8">
@@ -1790,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.006009252125773313</v>
+        <v>0.005999999999999998</v>
       </c>
     </row>
     <row r="9">
@@ -1807,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01343709624716425</v>
+        <v>0.01351542328847553</v>
       </c>
     </row>
     <row r="10">
@@ -1824,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02598290035987344</v>
+        <v>0.02639233895575676</v>
       </c>
     </row>
     <row r="11">
@@ -1841,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01931033114394699</v>
+        <v>0.01940503943710385</v>
       </c>
     </row>
   </sheetData>
@@ -1896,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4351570499987011</v>
+        <v>0.4361746830281742</v>
       </c>
     </row>
     <row r="3">
@@ -1910,7 +1910,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3149406296721927</v>
+        <v>0.3157890423588068</v>
       </c>
     </row>
     <row r="4">
@@ -1924,7 +1924,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5373415199439492</v>
+        <v>0.5381225776204775</v>
       </c>
     </row>
     <row r="5">
@@ -1938,7 +1938,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4975890094848109</v>
+        <v>0.4987906758790127</v>
       </c>
     </row>
     <row r="6">
@@ -1952,7 +1952,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3229186351756835</v>
+        <v>0.3241463999621798</v>
       </c>
     </row>
     <row r="7">
@@ -1966,7 +1966,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2741956749545512</v>
+        <v>0.2741279449337248</v>
       </c>
     </row>
     <row r="8">
@@ -1980,7 +1980,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2266725613695543</v>
+        <v>0.2264675296970426</v>
       </c>
     </row>
     <row r="9">
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2156155095295358</v>
+        <v>0.2152965150799589</v>
       </c>
     </row>
     <row r="10">
@@ -2008,7 +2008,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1996544648999615</v>
+        <v>0.1993508173286767</v>
       </c>
     </row>
     <row r="11">
@@ -2022,7 +2022,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4256774600371249</v>
+        <v>0.4248273930347688</v>
       </c>
     </row>
     <row r="12">
@@ -2036,7 +2036,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3044824945272546</v>
+        <v>0.303509595157636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BAU vs GES plot added
</commit_message>
<xml_diff>
--- a/protect_baltic/src/data/example/exampleResults.xlsx
+++ b/protect_baltic/src/data/example/exampleResults.xlsx
@@ -11,14 +11,16 @@
     <sheet name="PressureError" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="TPLMean" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="TPLError" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="ThresholdsMean" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="ThresholdsError" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="MeasureEffectsMean" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="MeasureEffectsError" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="ActivityContributionsMean" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="ActivityContributionsError" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="PressureContributionsMean" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="PressureContributionsError" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="TPLRedMean" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TPLRedError" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ThresholdsMean" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="ThresholdsError" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="MeasureEffectsMean" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="MeasureEffectsError" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="ActivityContributionsMean" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="ActivityContributionsError" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="PressureContributionsMean" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="PressureContributionsError" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,10 +464,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7113447999999999</v>
+        <v>0.7104478599999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.587032</v>
+        <v>0.5863744</v>
       </c>
     </row>
     <row r="3">
@@ -473,10 +475,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6096956486</v>
+        <v>0.6091678571999999</v>
       </c>
       <c r="C3" t="n">
-        <v>0.499592544</v>
+        <v>0.4982488879999999</v>
       </c>
     </row>
     <row r="4">
@@ -484,10 +486,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5250332</v>
+        <v>0.5244802</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4322551999999999</v>
+        <v>0.4319471999999999</v>
       </c>
     </row>
     <row r="5">
@@ -495,10 +497,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9643600000000001</v>
+        <v>0.96445</v>
       </c>
       <c r="C5" t="n">
-        <v>0.90496</v>
+        <v>0.9052</v>
       </c>
     </row>
     <row r="6">
@@ -506,7 +508,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8904</v>
+        <v>0.8888</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -518,6 +520,222 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>measure</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pressure</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>state</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>reduction</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.02757011264233629</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.03732886878066954</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.01916304313573974</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.02840970100355002</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.04363484845854286</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>31</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0407376429798725</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>11</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.005426273532033233</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.01343709624716425</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.02586288632169443</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.01940503943710385</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -564,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.009833094909913095</v>
+        <v>0.4353709447657666</v>
       </c>
     </row>
     <row r="3">
@@ -578,7 +796,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01503795225662456</v>
+        <v>0.3149535406205394</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.008203096626521822</v>
+        <v>0.537820513933705</v>
       </c>
     </row>
     <row r="5">
@@ -606,7 +824,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01231084081331761</v>
+        <v>0.4976291152974738</v>
       </c>
     </row>
     <row r="6">
@@ -620,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01217620155530652</v>
+        <v>0.3229186351756835</v>
       </c>
     </row>
     <row r="7">
@@ -634,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0004063846268960041</v>
+        <v>0.2741960557765753</v>
       </c>
     </row>
     <row r="8">
@@ -648,7 +866,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>0.001230300045353961</v>
+        <v>0.2266758623690024</v>
       </c>
     </row>
     <row r="9">
@@ -662,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.004203198890535038</v>
+        <v>0.2153909406335796</v>
       </c>
     </row>
     <row r="10">
@@ -676,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>0.005436662274549129</v>
+        <v>0.1996338886307541</v>
       </c>
     </row>
     <row r="11">
@@ -690,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01532015968747565</v>
+        <v>0.4243513200229904</v>
       </c>
     </row>
     <row r="12">
@@ -704,7 +922,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01390568315370264</v>
+        <v>0.3030761271457288</v>
       </c>
     </row>
   </sheetData>
@@ -712,7 +930,202 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Pressure</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>area_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>contribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.01014197888712356</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01521907032341857</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.008091062664235201</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.01234415070474169</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="n">
+        <v>31</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0122240578778499</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>11</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0003672140780737263</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>11</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.001109961089229045</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.004110878711824123</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.005296580315298724</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.01508633229707283</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01374218655893042</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -761,7 +1174,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.6727549802662831</v>
+        <v>0.6733643305958064</v>
       </c>
     </row>
     <row r="3">
@@ -777,7 +1190,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.2113769774816732</v>
+        <v>0.2107844914687276</v>
       </c>
     </row>
     <row r="4">
@@ -793,7 +1206,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.1158680422520436</v>
+        <v>0.1158511779354658</v>
       </c>
     </row>
     <row r="5">
@@ -809,7 +1222,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.83236812445981</v>
+        <v>0.8324256646460757</v>
       </c>
     </row>
     <row r="6">
@@ -825,7 +1238,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.1676318755401902</v>
+        <v>0.1675743353539245</v>
       </c>
     </row>
     <row r="7">
@@ -841,7 +1254,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.6343263002050215</v>
+        <v>0.6343802280772807</v>
       </c>
     </row>
     <row r="8">
@@ -857,7 +1270,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.250559293105184</v>
+        <v>0.2506832541763876</v>
       </c>
     </row>
     <row r="9">
@@ -873,7 +1286,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.1151144066897944</v>
+        <v>0.1149365177463316</v>
       </c>
     </row>
     <row r="10">
@@ -889,7 +1302,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.8352891734856789</v>
+        <v>0.8350453726687176</v>
       </c>
     </row>
     <row r="11">
@@ -905,7 +1318,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.1647108265143212</v>
+        <v>0.1649546273312825</v>
       </c>
     </row>
   </sheetData>
@@ -913,7 +1326,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -962,7 +1375,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.009322458761353375</v>
+        <v>0.009510175671527276</v>
       </c>
     </row>
     <row r="3">
@@ -978,7 +1391,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.009657071528972789</v>
+        <v>0.009678670512401224</v>
       </c>
     </row>
     <row r="4">
@@ -994,7 +1407,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.001632923101321011</v>
+        <v>0.001698509841188197</v>
       </c>
     </row>
     <row r="5">
@@ -1010,7 +1423,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.002487358973910752</v>
+        <v>0.002540880845765818</v>
       </c>
     </row>
     <row r="6">
@@ -1026,7 +1439,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.002487358973910721</v>
+        <v>0.002540880845765786</v>
       </c>
     </row>
     <row r="7">
@@ -1042,7 +1455,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.008045319065386506</v>
+        <v>0.008098823444570016</v>
       </c>
     </row>
     <row r="8">
@@ -1058,7 +1471,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.006492128472678519</v>
+        <v>0.006519183762071175</v>
       </c>
     </row>
     <row r="9">
@@ -1074,7 +1487,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.001944735896859549</v>
+        <v>0.002023963877862534</v>
       </c>
     </row>
     <row r="10">
@@ -1090,7 +1503,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.004606348893236272</v>
+        <v>0.004644754863739785</v>
       </c>
     </row>
     <row r="11">
@@ -1106,7 +1519,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.004606348893236218</v>
+        <v>0.004644754863739737</v>
       </c>
     </row>
   </sheetData>
@@ -1146,10 +1559,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.01215713906410551</v>
+        <v>0.01250220420132386</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01224750253725224</v>
+        <v>0.01239360619674516</v>
       </c>
     </row>
     <row r="3">
@@ -1157,10 +1570,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.009344207559866452</v>
+        <v>0.009272534382697163</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01188433385159427</v>
+        <v>0.01207069338012996</v>
       </c>
     </row>
     <row r="4">
@@ -1168,10 +1581,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.01444813800214024</v>
+        <v>0.01416654778679534</v>
       </c>
       <c r="C4" t="n">
-        <v>0.008498693898084178</v>
+        <v>0.008378658875447252</v>
       </c>
     </row>
     <row r="5">
@@ -1179,10 +1592,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0005400000000000001</v>
+        <v>0.0004883646178829976</v>
       </c>
       <c r="C5" t="n">
-        <v>0.001439999999999995</v>
+        <v>0.001302305647687974</v>
       </c>
     </row>
     <row r="6">
@@ -1190,7 +1603,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="n">
-        <v>0.01626666666666667</v>
+        <v>0.016295057191949</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -1233,10 +1646,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6131565049253417</v>
+        <v>0.6121994756205629</v>
       </c>
       <c r="C2" t="n">
-        <v>0.503246469473797</v>
+        <v>0.5026812125079263</v>
       </c>
     </row>
     <row r="3">
@@ -1244,10 +1657,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6223306234372835</v>
+        <v>0.6217556974094574</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5057565134872066</v>
+        <v>0.5045248084005899</v>
       </c>
     </row>
   </sheetData>
@@ -1287,10 +1700,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.008708835448271574</v>
+        <v>0.008842711549328825</v>
       </c>
       <c r="C2" t="n">
-        <v>0.007163802701522741</v>
+        <v>0.007217380464688405</v>
       </c>
     </row>
     <row r="3">
@@ -1298,10 +1711,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.00923368994353385</v>
+        <v>0.009196773415228468</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01066197055715727</v>
+        <v>0.01078845116166765</v>
       </c>
     </row>
   </sheetData>
@@ -1341,10 +1754,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5110000000000001</v>
+        <v>0.387800524379437</v>
       </c>
       <c r="C2" t="n">
-        <v>0.512</v>
+        <v>0.4973187874920737</v>
       </c>
     </row>
     <row r="3">
@@ -1352,10 +1765,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5399999999999999</v>
+        <v>0.3782443025905426</v>
       </c>
       <c r="C3" t="n">
-        <v>0.575</v>
+        <v>0.4954751915994101</v>
       </c>
     </row>
   </sheetData>
@@ -1395,10 +1808,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.01303414319734478</v>
+        <v>0.008842711549328822</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01364632632697249</v>
+        <v>0.007217380464688408</v>
       </c>
     </row>
     <row r="3">
@@ -1406,10 +1819,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.08481352093465602</v>
+        <v>0.00919677341522847</v>
       </c>
       <c r="C3" t="n">
-        <v>0.08709190547921203</v>
+        <v>0.01078845116166765</v>
       </c>
     </row>
   </sheetData>
@@ -1418,6 +1831,114 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5110000000000001</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.512</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5389999999999999</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5760000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01303414319734478</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.01364632632697249</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.08510712204170826</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.08740963587868585</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1472,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.411</v>
+        <v>0.413</v>
       </c>
     </row>
     <row r="3">
@@ -1506,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.354</v>
+        <v>0.355</v>
       </c>
     </row>
     <row r="5">
@@ -1523,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.227</v>
+        <v>0.226</v>
       </c>
     </row>
     <row r="6">
@@ -1540,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.344</v>
+        <v>0.348</v>
       </c>
     </row>
     <row r="7">
@@ -1557,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.274</v>
+        <v>0.278</v>
       </c>
     </row>
     <row r="8">
@@ -1574,7 +2095,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
     </row>
     <row r="9">
@@ -1591,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.424</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="10">
@@ -1608,7 +2129,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.599</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11">
@@ -1626,417 +2147,6 @@
       </c>
       <c r="E11" t="n">
         <v>0.659</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>measure</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>activity</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pressure</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>reduction</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.0267685553505518</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.03732886878066954</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.01967513941783161</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.02808914381037628</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.04292629341868066</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>31</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.04066666666666666</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="n">
-        <v>11</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.005999999999999998</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>3</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.01351542328847553</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.02639233895575676</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>3</v>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="n">
-        <v>3</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.01940503943710385</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Pressure</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>area_id</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>contribution</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.4361746830281742</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.3157890423588068</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.5381225776204775</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.4987906758790127</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="n">
-        <v>31</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.3241463999621798</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>11</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.2741279449337248</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>11</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.2264675296970426</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.2152965150799589</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.1993508173286767</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.4248273930347688</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.303509595157636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>